<commit_message>
Fix minValue restriction error
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -2276,7 +2276,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-08-04T07:36:40-07:00</t>
+    <t>2023-08-11T13:12:31-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2521,14 +2521,14 @@
     <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_model'!$A$1:$A$30</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
@@ -2544,15 +2544,15 @@
     <dataValidation type="list" sqref="V2:V1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'scan_direction'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>1</formula1>
       <formula2/>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>1</formula1>
       <formula2/>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>

</xml_diff>

<commit_message>
Updating the categorical value IRIs
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="691">
   <si>
     <t>parent_id</t>
   </si>
@@ -1823,12 +1823,6 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C449</t>
   </si>
   <si>
-    <t>N-glycan</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_59520</t>
-  </si>
-  <si>
     <t>Endogenous fluorophores</t>
   </si>
   <si>
@@ -2276,7 +2270,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-08-11T13:12:31-07:00</t>
+    <t>2023-09-08T20:50:42-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2439,55 +2433,55 @@
         <v>528</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="O1" t="s" s="1">
+        <v>655</v>
+      </c>
+      <c r="P1" t="s" s="1">
+        <v>656</v>
+      </c>
+      <c r="Q1" t="s" s="1">
         <v>657</v>
       </c>
-      <c r="P1" t="s" s="1">
+      <c r="R1" t="s" s="1">
         <v>658</v>
       </c>
-      <c r="Q1" t="s" s="1">
+      <c r="S1" t="s" s="1">
         <v>659</v>
       </c>
-      <c r="R1" t="s" s="1">
+      <c r="T1" t="s" s="1">
         <v>660</v>
       </c>
-      <c r="S1" t="s" s="1">
+      <c r="U1" t="s" s="1">
         <v>661</v>
       </c>
-      <c r="T1" t="s" s="1">
-        <v>662</v>
-      </c>
-      <c r="U1" t="s" s="1">
-        <v>663</v>
-      </c>
       <c r="V1" t="s" s="1">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="W1" t="s" s="1">
+        <v>679</v>
+      </c>
+      <c r="X1" t="s" s="1">
+        <v>680</v>
+      </c>
+      <c r="Y1" t="s" s="1">
         <v>681</v>
       </c>
-      <c r="X1" t="s" s="1">
+      <c r="Z1" t="s" s="1">
         <v>682</v>
-      </c>
-      <c r="Y1" t="s" s="1">
-        <v>683</v>
-      </c>
-      <c r="Z1" t="s" s="1">
-        <v>684</v>
       </c>
     </row>
     <row r="2">
@@ -2495,7 +2489,7 @@
         <v>462</v>
       </c>
       <c r="Z2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -2510,7 +2504,7 @@
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
@@ -2533,7 +2527,7 @@
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$5</formula1>
+      <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
@@ -2565,7 +2559,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2593,22 +2587,6 @@
       </c>
       <c r="B3" t="s">
         <v>652</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>653</v>
-      </c>
-      <c r="B4" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>655</v>
-      </c>
-      <c r="B5" t="s">
-        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -2626,18 +2604,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -2655,34 +2633,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B3" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -2700,34 +2678,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -2751,16 +2729,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C1" t="s">
         <v>687</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>689</v>
-      </c>
-      <c r="D1" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="2">
@@ -2768,13 +2746,13 @@
         <v>462</v>
       </c>
       <c r="B2" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2" t="s">
         <v>688</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>690</v>
-      </c>
-      <c r="D2" t="s">
-        <v>692</v>
       </c>
     </row>
   </sheetData>
@@ -4903,7 +4881,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4987,14 +4965,6 @@
       </c>
       <c r="B10" t="s">
         <v>548</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>549</v>
-      </c>
-      <c r="B11" t="s">
-        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -5012,18 +4982,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -5041,114 +5011,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B7" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B9" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B10" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B11" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -5166,242 +5136,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B6" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B7" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B9" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B10" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B11" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B13" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B14" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B15" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B16" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B17" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B20" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B21" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B22" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B23" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B24" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B25" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B26" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B27" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B28" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B29" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B30" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -5419,42 +5389,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the other assays
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -31,11 +31,11 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) HuBMAP ID (e.g., HBM765.TRHD.452) of the sample (i.e., block, section
-or suspension) used to perform this assay. For example, for a RNAseq assay, the
-parent would be the suspension, whereas this would be the HuBMAP ID of a section
-for one of the imaging assays. If an assay comes from multiple parent samples
-then this should be a comma separated list.</t>
+        <t>(Required) HuBMAP ID of the sample (i.e., block, section or suspension) used to
+perform this assay. For example, for a RNAseq assay, the parent would be the
+suspension, whereas this would be the HuBMAP ID of a section for one of the
+imaging assays. If an assay comes from multiple parent samples then this should
+be a comma separated list. Example: HBM765.TRHD.452</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
@@ -54,7 +54,8 @@
 procurment and preparation. For example for an imaging assay, the protocol might
 include staining of a section through the creation of an OME-TIFF file. In this
 case the protocol would include any image processing steps required to create
-the OME-TIFF file.</t>
+the OME-TIFF file. Example:
+https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
@@ -70,7 +71,8 @@
     <comment ref="F1" authorId="1">
       <text>
         <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay. The CODEX analyte is protein.</t>
+detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
+protein.</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
@@ -186,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="246">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -224,6 +226,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
   </si>
   <si>
+    <t>scATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000247</t>
+  </si>
+  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
@@ -236,30 +244,30 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
   </si>
   <si>
-    <t>snATAC-seq</t>
+    <t>scRNAseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000248</t>
+  </si>
+  <si>
+    <t>Xenium</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
+  </si>
+  <si>
+    <t>snATACseq</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000183</t>
   </si>
   <si>
-    <t>Xenium</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
-  </si>
-  <si>
     <t>Molecular Cartography</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>scRNA-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000248</t>
-  </si>
-  <si>
     <t>CosMx</t>
   </si>
   <si>
@@ -302,114 +310,108 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000160</t>
   </si>
   <si>
-    <t>snRNA-seq</t>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>NanoDESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000203</t>
+  </si>
+  <si>
+    <t>GeoMx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000216</t>
+  </si>
+  <si>
+    <t>RNAseq (bulk)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000212</t>
+  </si>
+  <si>
+    <t>MALDI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
+  </si>
+  <si>
+    <t>RNAseq (GeoMx)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000214</t>
+  </si>
+  <si>
+    <t>Histology</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000197</t>
+  </si>
+  <si>
+    <t>Enhanced Stimulated Raman Spectroscopy (SRS)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
+  </si>
+  <si>
+    <t>ATACseq (bulk)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000210</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>LC-MS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000194</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>snRNAseq</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000184</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
-  </si>
-  <si>
-    <t>NanoDESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000203</t>
-  </si>
-  <si>
-    <t>GeoMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000216</t>
-  </si>
-  <si>
-    <t>RNAseq (bulk)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000212</t>
-  </si>
-  <si>
-    <t>MALDI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
-  </si>
-  <si>
-    <t>RNAseq (GeoMx)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000214</t>
-  </si>
-  <si>
-    <t>Histology</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000197</t>
-  </si>
-  <si>
-    <t>scATAC-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000247</t>
-  </si>
-  <si>
-    <t>Enhanced Stimulated Raman Spectroscopy (SRS)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
-  </si>
-  <si>
-    <t>ATACseq (bulk)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000210</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
-    <t>LC-MS</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000194</t>
-  </si>
-  <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>Visium</t>
   </si>
   <si>
@@ -425,6 +427,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>Nucleic acid and protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000273</t>
+  </si>
+  <si>
     <t>Fluorochrome</t>
   </si>
   <si>
@@ -596,18 +604,24 @@
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>Zeiss Lightsheet 7</t>
+    <t>Axio Observer 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023694</t>
+  </si>
+  <si>
+    <t>IN Cell Analyzer 2200</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023616</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024448</t>
   </si>
   <si>
-    <t>IN Cell Analyzer 2200</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023616</t>
-  </si>
-  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -626,6 +640,18 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>Axio Observer 5</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023692</t>
+  </si>
+  <si>
+    <t>Axio Observer 3</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023693</t>
+  </si>
+  <si>
     <t>HiSeq 2500</t>
   </si>
   <si>
@@ -668,36 +694,18 @@
     <t>https://identifiers.org/RRID:SCR_023610</t>
   </si>
   <si>
-    <t>Zeiss Axio Observer 5</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023692</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Zeiss Axio Observer 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023694</t>
-  </si>
-  <si>
     <t>QTRAP 5500</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_020517</t>
   </si>
   <si>
-    <t>Zeiss Axio Observer 3</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023693</t>
-  </si>
-  <si>
     <t>BZ-X800</t>
   </si>
   <si>
@@ -911,7 +919,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-03T15:12:02-07:00</t>
+    <t>2023-10-06T19:30:51-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1054,63 +1062,63 @@
         <v>76</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1127,7 @@
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$10</formula1>
+      <formula1>'analyte_class'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
@@ -1182,42 +1190,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1235,42 +1243,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1294,30 +1302,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1628,7 +1636,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1712,6 +1720,14 @@
       </c>
       <c r="B10" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1729,12 +1745,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1752,114 +1768,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1877,258 +1893,258 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2146,42 +2162,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2199,26 +2215,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2236,12 +2252,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix missing dropdown option when the column name is too long in Excel
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="277">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -489,6 +489,18 @@
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
+    <t>In-House</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
+    <t>BGI Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024848</t>
+  </si>
+  <si>
     <t>Resolve Biosciences</t>
   </si>
   <si>
@@ -531,6 +543,18 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Akoya Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023774</t>
+  </si>
+  <si>
+    <t>Evident Scientific (Olympus)</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024782</t>
+  </si>
+  <si>
     <t>Keyence</t>
   </si>
   <si>
@@ -567,6 +591,12 @@
     <t>https://identifiers.org/RRID:SCR_010233</t>
   </si>
   <si>
+    <t>Motic</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024856</t>
+  </si>
+  <si>
     <t>Ionpath</t>
   </si>
   <si>
@@ -600,6 +630,12 @@
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
@@ -618,18 +654,42 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>DM6 B</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024857</t>
+  </si>
+  <si>
     <t>NanoZoomer 2.0-HT</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_021658</t>
   </si>
   <si>
+    <t>Phenocycler-Fusion 2.0</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023773</t>
+  </si>
+  <si>
     <t>Lightsheet 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024448</t>
   </si>
   <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -654,6 +714,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>VS200 Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024783</t>
+  </si>
+  <si>
     <t>Axio Observer 5</t>
   </si>
   <si>
@@ -714,6 +780,12 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
     <t>QTRAP 5500</t>
   </si>
   <si>
@@ -948,7 +1020,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-24T09:41:35-08:00</t>
+    <t>2024-01-29T14:09:18-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1051,29 +1123,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.6875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="6.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="23.45703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="12.28515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="12.66796875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="10.8984375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="28.46484375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="27.87109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="28.5625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="27.40234375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="47.64453125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="46.48828125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="14" width="16.90625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" style="15" width="9.81640625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="15.234375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="30.79296875" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="7.8125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="16.65625" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="13.859375" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="19.734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="17.2421875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="30.83203125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" style="24" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="14.39453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="20.234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="10.59765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="10.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="9.40234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="24.5546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="24.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="24.63671875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="23.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="41.1015625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="40.1015625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="14" width="14.5859375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" style="15" width="8.46484375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="13.14453125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="26.5625" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="6.7421875" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="14.3671875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="11.953125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="17.0234375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="14.875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="26.59765625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" style="24" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1099,60 +1171,60 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>244</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2">
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="W2" t="s">
-        <v>245</v>
+      <c r="W2" t="s" s="24">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1167,10 +1239,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$14</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$38</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1184,7 +1256,7 @@
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
+      <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
@@ -1223,43 +1295,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
+      <c r="A1" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>247</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" t="s">
-        <v>225</v>
+      <c r="A2" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>249</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" t="s">
-        <v>227</v>
+      <c r="A3" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>251</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" t="s">
-        <v>229</v>
+      <c r="A4" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>253</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B5" t="s">
-        <v>231</v>
+      <c r="A5" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1276,43 +1348,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" t="s">
-        <v>234</v>
+      <c r="A1" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>258</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" t="s">
-        <v>236</v>
+      <c r="A2" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>260</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" t="s">
-        <v>238</v>
+      <c r="A3" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>262</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>226</v>
-      </c>
-      <c r="B4" t="s">
-        <v>227</v>
+      <c r="A4" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>251</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" t="s">
-        <v>240</v>
+      <c r="A5" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1328,38 +1400,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="17.55078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="79.94921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="15.140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.96484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" t="s">
-        <v>251</v>
+      <c r="A1" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>273</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>275</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D2" t="s">
-        <v>252</v>
+      <c r="B2" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -1376,266 +1448,266 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>51</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>55</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>57</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>59</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>61</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>65</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>67</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>69</v>
       </c>
     </row>
@@ -1653,90 +1725,90 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>72</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>74</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>76</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>80</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>82</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>86</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>88</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>90</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -1754,12 +1826,12 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>94</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>95</v>
       </c>
     </row>
@@ -1770,122 +1842,162 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>100</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>102</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>104</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>108</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>110</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>112</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>114</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>116</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>118</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>120</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>122</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>124</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1895,314 +2007,370 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" t="s">
-        <v>127</v>
+      <c r="A1" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>137</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
+      <c r="A2" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>139</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>131</v>
+      <c r="A3" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>141</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" t="s">
-        <v>133</v>
+      <c r="A4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>143</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" t="s">
-        <v>135</v>
+      <c r="A5" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>145</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>137</v>
+      <c r="A6" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>147</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" t="s">
-        <v>139</v>
+      <c r="A7" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>149</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>141</v>
+      <c r="A8" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>151</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
+      <c r="A9" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>153</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" t="s">
-        <v>145</v>
+      <c r="A10" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>155</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" t="s">
-        <v>147</v>
+      <c r="A11" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>157</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" t="s">
-        <v>149</v>
+      <c r="A12" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>159</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" t="s">
-        <v>151</v>
+      <c r="A13" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>161</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" t="s">
-        <v>153</v>
+      <c r="A14" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>163</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>155</v>
+      <c r="A15" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>165</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" t="s">
-        <v>157</v>
+      <c r="A16" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>167</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" t="s">
-        <v>159</v>
+      <c r="A17" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>169</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B18" t="s">
-        <v>161</v>
+      <c r="A18" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>171</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" t="s">
-        <v>163</v>
+      <c r="A19" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>173</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" t="s">
-        <v>165</v>
+      <c r="A20" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>175</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>166</v>
-      </c>
-      <c r="B21" t="s">
-        <v>167</v>
+      <c r="A21" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>177</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>168</v>
-      </c>
-      <c r="B22" t="s">
-        <v>169</v>
+      <c r="A22" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>179</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" t="s">
-        <v>171</v>
+      <c r="A23" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>181</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" t="s">
-        <v>173</v>
+      <c r="A24" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>183</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" t="s">
-        <v>175</v>
+      <c r="A25" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>185</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B26" t="s">
-        <v>177</v>
+      <c r="A26" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>187</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>178</v>
-      </c>
-      <c r="B27" t="s">
-        <v>179</v>
+      <c r="A27" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>189</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B28" t="s">
-        <v>181</v>
+      <c r="A28" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>191</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>182</v>
-      </c>
-      <c r="B29" t="s">
-        <v>183</v>
+      <c r="A29" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>193</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" t="s">
-        <v>185</v>
+      <c r="A30" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>195</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>186</v>
-      </c>
-      <c r="B31" t="s">
-        <v>187</v>
+      <c r="A31" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>197</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>188</v>
-      </c>
-      <c r="B32" t="s">
-        <v>189</v>
+      <c r="A32" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>190</v>
-      </c>
-      <c r="B33" t="s">
-        <v>191</v>
+      <c r="A33" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>201</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>192</v>
-      </c>
-      <c r="B34" t="s">
-        <v>193</v>
+      <c r="A34" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>203</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" t="s">
-        <v>195</v>
+      <c r="A35" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>205</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>196</v>
-      </c>
-      <c r="B36" t="s">
-        <v>197</v>
+      <c r="A36" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>207</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B37" t="s">
-        <v>199</v>
+      <c r="A37" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>209</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B38" t="s">
-        <v>201</v>
+      <c r="A38" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>212</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2219,43 +2387,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" t="s">
-        <v>205</v>
+      <c r="A1" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>229</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" t="s">
-        <v>207</v>
+      <c r="A2" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>231</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B3" t="s">
-        <v>209</v>
+      <c r="A3" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>233</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" t="s">
-        <v>211</v>
+      <c r="A4" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>235</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" t="s">
-        <v>213</v>
+      <c r="A5" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2272,27 +2440,27 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" t="s">
-        <v>207</v>
+      <c r="A1" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>231</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" t="s">
-        <v>209</v>
+      <c r="A2" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>233</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
+      <c r="A3" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2309,12 +2477,12 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>94</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Leica Microsystems' in the acquisition instrument vendor
Closes #27
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="299">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -306,6 +306,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -411,6 +417,12 @@
     <t>analyte_class</t>
   </si>
   <si>
+    <t>DNA + RNA</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -531,6 +543,12 @@
     <t>https://identifiers.org/RRID:SCR_023606</t>
   </si>
   <si>
+    <t>GE Healthcare</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_000004</t>
+  </si>
+  <si>
     <t>Sciex</t>
   </si>
   <si>
@@ -543,6 +561,12 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Leica Microsystems</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008960</t>
+  </si>
+  <si>
     <t>Akoya Biosciences</t>
   </si>
   <si>
@@ -585,6 +609,12 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
@@ -624,16 +654,142 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
+    <t>BZ-X810</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025160</t>
   </si>
   <si>
     <t>Axio Observer 7</t>
@@ -642,52 +798,34 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
     <t>DM6 B</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024857</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
     <t>Phenocycler-Fusion 2.0</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
+    <t>Aperio CS2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025111</t>
   </si>
   <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
@@ -702,18 +840,18 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -744,12 +882,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -762,40 +894,16 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
   </si>
   <si>
     <t>MIBIscope</t>
@@ -804,18 +912,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -828,36 +924,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1020,7 +1086,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-29T14:09:18-08:00</t>
+    <t>2024-04-01T14:45:46-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1162,61 +1228,61 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>268</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
@@ -1224,25 +1290,25 @@
         <v>14</v>
       </c>
       <c r="W2" t="s" s="24">
-        <v>269</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="15">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$51</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1296,42 +1362,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>247</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>249</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>251</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>253</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>255</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -1349,42 +1415,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>258</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>260</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>262</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>251</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>264</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -1408,16 +1474,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>275</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2">
@@ -1425,13 +1491,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>276</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1507,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1711,6 +1777,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1718,7 +1792,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1726,90 +1800,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1827,12 +1909,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1842,7 +1924,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1850,154 +1932,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2007,7 +2113,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2015,362 +2121,410 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>225</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2388,42 +2542,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>229</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>231</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>237</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2441,26 +2595,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>231</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2478,12 +2632,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introduce new analyte classes
New analyte classes: Collagen, Saturated lipid, Unsaturated lipid

Closes #48
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="309">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -258,6 +258,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
     <t>Visium (with probes)</t>
   </si>
   <si>
@@ -354,6 +360,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
   </si>
   <si>
+    <t>Resolve</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000384</t>
+  </si>
+  <si>
     <t>RNAseq</t>
   </si>
   <si>
@@ -435,22 +447,52 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000273</t>
   </si>
   <si>
+    <t>RNA</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C812</t>
+  </si>
+  <si>
+    <t>Metabolite</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C61154</t>
+  </si>
+  <si>
+    <t>Unsaturated Lipid</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000389</t>
+  </si>
+  <si>
+    <t>Saturated Lipid</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000388</t>
+  </si>
+  <si>
+    <t>Lipid</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C616</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17021</t>
+  </si>
+  <si>
     <t>Fluorochrome</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_51217</t>
   </si>
   <si>
-    <t>RNA</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C812</t>
-  </si>
-  <si>
-    <t>Metabolite</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C61154</t>
+    <t>Collagen</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C16447</t>
   </si>
   <si>
     <t>DNA</t>
@@ -477,27 +519,15 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_18154</t>
   </si>
   <si>
-    <t>Lipid</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C616</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17021</t>
-  </si>
-  <si>
     <t>is_targeted</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
@@ -546,7 +576,7 @@
     <t>GE Healthcare</t>
   </si>
   <si>
-    <t>https://identifiers.org/RRID:SCR_000004</t>
+    <t>https://identifiers.org/RRID:SCR_025461</t>
   </si>
   <si>
     <t>Sciex</t>
@@ -654,6 +684,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
+  </si>
+  <si>
     <t>MoticEasyScan One</t>
   </si>
   <si>
@@ -1002,6 +1038,12 @@
     <t>tile_configuration</t>
   </si>
   <si>
+    <t>Row-by-row</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000138</t>
+  </si>
+  <si>
     <t>Column-by-column</t>
   </si>
   <si>
@@ -1014,24 +1056,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000122</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
-  </si>
-  <si>
     <t>Snake-by-columns</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000110</t>
   </si>
   <si>
-    <t>Row-by-row</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000138</t>
-  </si>
-  <si>
     <t>scan_direction</t>
   </si>
   <si>
@@ -1041,18 +1071,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000111</t>
   </si>
   <si>
+    <t>Right-and-up</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000141</t>
+  </si>
+  <si>
     <t>Left-and-down</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000108</t>
   </si>
   <si>
-    <t>Right-and-up</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000141</t>
-  </si>
-  <si>
     <t>Right-and-down</t>
   </si>
   <si>
@@ -1086,7 +1116,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-01T14:45:46-07:00</t>
+    <t>2024-08-03T11:38:53-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1228,61 +1258,61 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2">
@@ -1290,16 +1320,16 @@
         <v>14</v>
       </c>
       <c r="W2" t="s" s="24">
-        <v>291</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="15">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$34</formula1>
+      <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$12</formula1>
+      <formula1>'analyte_class'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
@@ -1308,7 +1338,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$51</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1362,42 +1392,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>268</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>269</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -1415,42 +1445,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>283</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>284</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>272</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>273</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -1474,16 +1504,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>297</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
@@ -1491,13 +1521,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>298</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1537,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1785,6 +1815,22 @@
         <v>71</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1792,7 +1838,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1800,98 +1846,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>96</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1909,12 +1979,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1932,178 +2002,178 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2113,7 +2183,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2121,410 +2191,418 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>243</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>247</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2542,42 +2620,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2595,26 +2673,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2632,12 +2710,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new acquisition instrument models
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="359">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -936,6 +936,18 @@
     <t>https://identifiers.org/RRID:SCR_021660</t>
   </si>
   <si>
+    <t>timsTOF FleX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026925</t>
+  </si>
+  <si>
+    <t>timsTOF FleX MALDI-2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023615</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
@@ -1005,7 +1017,7 @@
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
-    <t>https://identifiers.org/RRID:SCR_023615</t>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000433</t>
   </si>
   <si>
     <t>TissueScope LE Slide Scanner</t>
@@ -1254,7 +1266,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:46:05-07:00</t>
+    <t>2025-05-12T10:12:32-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1408,49 +1420,49 @@
         <v>175</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2">
@@ -1458,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="W2" t="s" s="24">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -1476,7 +1488,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$66</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1538,34 +1550,34 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -1583,18 +1595,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3">
@@ -1607,18 +1619,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -1642,16 +1654,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2">
@@ -1659,13 +1671,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2413,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2857,26 +2869,26 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>149</v>
+        <v>288</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>150</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>290</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>291</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60">
@@ -2933,6 +2945,22 @@
       </c>
       <c r="B66" t="s" s="0">
         <v>305</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2950,42 +2978,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3003,26 +3031,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SFM metadata templates to use the updated field descriptions
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -31,163 +31,172 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"/TEST001-RK/" for this field. If there are multiple directory levels, use the
-format "/TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) This is the location of the antibodies.tsv file relative to the root
-of the top level of the upload directory structure. This path should begin with
-"." and would likely be something like "./extras/antibodies.tsv".</t>
+        <t>(Required) The path to the antibodies.tsv file relative to the root directory of
+the upload structure. This path should start with "." and is typically formatted
+as "./extras/antibodies.tsv". Example: ./extras/antibodies.tsv</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>Depending on if the acquisition instrument was a microscope, slide scanner, etc.
-will indicate whether or not any level of preprocessing was required to assemble
-the image (e.g., fusing image tiles) .</t>
+        <t>Indicates whether image preprocessing is necessary based on the type of
+acquisition instrument used, such as a microscope or slide scanner. This may
+involve steps like fusing image tiles to assemble the complete image. Example:
+Yes</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>A unique ID denoting the slide used. This allows users the ability to determine
-which tissue sections were processed together on the same slide. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+        <t>The unique identifier assigned to each slide, enabling users to determine which
+tissue sections were processed together on the same slide. It is recommended
+that data providers prefix the ID with the center name to prevent overlapping
+values across different centers. Example: VAN0071-PA-1-1_AF</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>This is how the tiles are configured for stitching.</t>
+        <t>The configuration of tiles used for stitching in the assay process. If no tile
+configuration is applicable, enter "Not applicable". Example: Row-by-row</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>This is the direction of imaging, which is required for stitching.</t>
+        <t>The direction of imaging, which is necessary for the stitching process. Example:
+Left-and-down</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>This is how many columns used in stitching. This is sometimes referred to as the
-grid size x.</t>
+        <t>The number of columns used in the stitching process of a tiled image, often
+referred to as the grid size in the x-dimension. Example: 5</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>This is the total number of raw (tiled) images captured, that are to be stitched
-together.</t>
+        <t>The total number of raw tiled images captured, which are intended to be stitched
+together. Example: 75</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>The amount of overlap between tiled images. This is the set point, where as
-during image acquisition there will be slight variations due to stage
-registration.</t>
+        <t>The intended percentage of overlap between tiled images. This value serves as
+the set point, although slight variations may occur during image acquisition due
+to stage registration. Example: 5</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -196,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="402">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -222,34 +231,172 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -258,36 +405,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -318,16 +435,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -336,30 +447,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -390,18 +483,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -414,12 +495,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -432,34 +507,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -723,12 +780,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -876,6 +945,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -996,6 +1071,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1086,6 +1167,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1116,6 +1200,12 @@
     <t>https://identifiers.org/RRID:SCR_027095</t>
   </si>
   <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1128,6 +1218,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1152,6 +1248,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1302,7 +1404,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-24T10:41:15-07:00</t>
+    <t>2025-10-23T10:17:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1444,75 +1546,75 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>322</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>323</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>337</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>338</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>339</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>340</v>
+        <v>371</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>341</v>
+        <v>372</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>350</v>
+        <v>381</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>359</v>
+        <v>390</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>360</v>
+        <v>391</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>361</v>
+        <v>392</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>362</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="W2" t="s" s="24">
-        <v>363</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="15">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1521,10 +1623,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$28</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$71</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1578,42 +1680,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>343</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>344</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>345</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>346</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>347</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>349</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -1631,42 +1733,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>384</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>356</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>357</v>
+        <v>388</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>358</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -1690,30 +1792,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>364</v>
+        <v>395</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>365</v>
+        <v>396</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>367</v>
+        <v>398</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>369</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>366</v>
+        <v>397</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>368</v>
+        <v>399</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>370</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -1723,7 +1825,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2063,6 +2165,70 @@
       </c>
       <c r="B42" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2080,130 +2246,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2221,12 +2387,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2236,7 +2402,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2244,226 +2410,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>180</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2655,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2481,570 +2663,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>199</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>203</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>223</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>227</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>237</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>243</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>255</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>259</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>281</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>289</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>300</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>301</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>155</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>156</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>303</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>306</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>307</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>309</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>313</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>315</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>317</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>319</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>321</v>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3062,42 +3292,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>327</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>329</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>331</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>332</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>333</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3115,26 +3345,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>327</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>329</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>331</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3152,12 +3382,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added optional non_global_files field to AF and Enhanced SRS spec
Closes #140
</commit_message>
<xml_diff>
--- a/af/latest/af.xlsx
+++ b/af/latest/af.xlsx
@@ -195,6 +195,21 @@
     </comment>
     <comment ref="W1" authorId="1">
       <text>
+        <t>Specifies a semicolon-separated list of non-global files that are to be included
+in the dataset. The file paths assume that the files are located in the
+"TOP/non-global/" directory. For instance, if the file is located at
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson, the value for
+this field would be "./lab_processed/images/1-tissue-boundary.geojson". Once
+ingested, these files will be copied to their appropriate locations within the
+respective dataset directory tree. This field is intended for internal HuBMAP
+processing. Examples for GeoMx and PhenoCycler are provided in the File
+Locations documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee
+Example: ./lab_processed/images/1-tissue-boundary.geojson</t>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="1">
+      <text>
         <t>(Required) The unique string identifier for the metadata specification version,
 which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -205,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="431">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -309,6 +324,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
+    <t>iCLAP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000479</t>
+  </si>
+  <si>
     <t>seqFISH</t>
   </si>
   <si>
@@ -507,6 +528,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
   </si>
   <si>
+    <t>Raman Imaging</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000475</t>
+  </si>
+  <si>
     <t>RNAseq (with probes)</t>
   </si>
   <si>
@@ -519,6 +546,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
+    <t>STARmap</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000476</t>
+  </si>
+  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -546,6 +579,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>Lipid + metabolite + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000478</t>
+  </si>
+  <si>
     <t>RNA + protein</t>
   </si>
   <si>
@@ -732,6 +771,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -792,6 +837,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -921,6 +972,18 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -963,6 +1026,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1089,6 +1158,18 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1230,6 +1311,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -1398,6 +1485,9 @@
     <t>intended_tile_overlap_percentage</t>
   </si>
   <si>
+    <t>non_global_files</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1416,7 +1506,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-20T09:36:20-08:00</t>
+    <t>2026-01-29T11:19:29-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1475,7 +1565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1503,6 +1593,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1513,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1541,7 +1632,8 @@
     <col min="20" max="20" style="21" width="17.0234375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" style="22" width="14.875" customWidth="true" bestFit="true"/>
     <col min="22" max="22" style="23" width="26.59765625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" style="24" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" style="24" width="13.33984375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" style="25" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1558,87 +1650,90 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>357</v>
+        <v>381</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>369</v>
+        <v>393</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>370</v>
+        <v>394</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>372</v>
+        <v>396</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>373</v>
+        <v>397</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>374</v>
+        <v>398</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>375</v>
+        <v>399</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>376</v>
+        <v>400</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>385</v>
+        <v>409</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>397</v>
+        <v>421</v>
+      </c>
+      <c r="X1" t="s" s="1">
+        <v>422</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>62</v>
-      </c>
-      <c r="W2" t="s" s="24">
-        <v>398</v>
+        <v>64</v>
+      </c>
+      <c r="X2" t="s" s="25">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="15">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$51</formula1>
+      <formula1>'dataset_type'!$A$1:$A$54</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$17</formula1>
+      <formula1>'analyte_class'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$32</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$83</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1692,42 +1787,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>401</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>403</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>383</v>
+        <v>407</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>384</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -1745,42 +1840,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>386</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>387</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>389</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>391</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>392</v>
+        <v>416</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>393</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -1804,30 +1899,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>404</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>405</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1932,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2251,6 +2346,30 @@
         <v>105</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2258,7 +2377,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2266,138 +2385,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2415,12 +2542,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2430,7 +2557,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2438,242 +2565,258 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>204</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2826,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2691,618 +2834,666 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>239</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>241</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>281</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>289</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>323</v>
+        <v>335</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>70</v>
+        <v>336</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>324</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>330</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>175</v>
+        <v>344</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>176</v>
+        <v>345</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>332</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>334</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>336</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>338</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>339</v>
+        <v>185</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>340</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>342</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>344</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>352</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>356</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3320,42 +3511,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>365</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>366</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>368</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3373,26 +3564,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>364</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>365</v>
+        <v>389</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>366</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -3410,12 +3601,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>